<commit_message>
sua va them get_core0, get_core1 + def student() option = 0 1
</commit_message>
<xml_diff>
--- a/score/GIS_DC/GIS_DC.xlsx
+++ b/score/GIS_DC/GIS_DC.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Python\Tiểu luận - NMLT\score\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\python\TL\TLGiang\score\GIS_DC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194914C1-7ABC-4EAC-8DA8-9D426B3FCB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="11016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,16 +394,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F21"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -444,7 +446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -464,7 +466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -484,7 +486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -504,7 +506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -524,7 +526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -544,7 +546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -564,7 +566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -584,7 +586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -604,7 +606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -624,7 +626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -644,7 +646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -664,7 +666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -684,7 +686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -704,7 +706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -724,7 +726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -744,7 +746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -764,7 +766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -784,7 +786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -804,7 +806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
pull len de test
</commit_message>
<xml_diff>
--- a/score/GIS_DC/GIS_DC.xlsx
+++ b/score/GIS_DC/GIS_DC.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\python\TL\TLGiang\score\GIS_DC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PYTHON\Tieu_luan\score\GIS_DC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993FFF63-2A4A-4930-ADE9-E84FF97E2E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="11016" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gi01A" sheetId="1" r:id="rId1"/>
@@ -620,7 +621,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -931,20 +932,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -964,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -984,7 +985,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1024,7 +1025,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1104,7 +1105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1124,7 +1125,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1164,7 +1165,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1184,7 +1185,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1204,7 +1205,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1224,7 +1225,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1244,7 +1245,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1264,7 +1265,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1284,7 +1285,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1304,7 +1305,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1324,7 +1325,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1344,7 +1345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1364,7 +1365,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1384,7 +1385,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1404,7 +1405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1424,7 +1425,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1444,7 +1445,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1464,7 +1465,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1484,7 +1485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1504,7 +1505,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1524,7 +1525,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1544,7 +1545,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1564,7 +1565,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1584,7 +1585,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1644,7 +1645,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1664,7 +1665,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1684,7 +1685,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1704,7 +1705,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1724,7 +1725,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1744,7 +1745,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1764,7 +1765,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1784,7 +1785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1804,7 +1805,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1824,7 +1825,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1864,7 +1865,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1884,7 +1885,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1904,7 +1905,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1924,7 +1925,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1944,7 +1945,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1964,7 +1965,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1984,7 +1985,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2025,7 +2026,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:D54">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D54">
     <sortCondition ref="B2:B54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2033,19 +2034,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2065,7 +2066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2085,7 +2086,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2105,7 +2106,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2145,7 +2146,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2165,7 +2166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2185,7 +2186,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2205,7 +2206,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2225,7 +2226,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2265,7 +2266,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2285,7 +2286,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2305,7 +2306,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2325,7 +2326,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2345,7 +2346,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2365,7 +2366,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2385,7 +2386,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2405,7 +2406,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2425,7 +2426,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2445,7 +2446,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2465,7 +2466,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2485,7 +2486,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2505,7 +2506,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2525,7 +2526,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2545,7 +2546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2585,7 +2586,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2605,7 +2606,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2625,7 +2626,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2645,7 +2646,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2665,7 +2666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2685,7 +2686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2705,7 +2706,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2725,7 +2726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2745,7 +2746,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2765,7 +2766,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2785,7 +2786,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2825,7 +2826,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2845,7 +2846,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2865,7 +2866,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2885,7 +2886,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2905,7 +2906,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2925,7 +2926,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2945,7 +2946,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2965,7 +2966,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2985,7 +2986,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3005,7 +3006,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3025,7 +3026,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3045,7 +3046,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3065,7 +3066,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3086,7 +3087,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:D52">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D52">
     <sortCondition ref="B2:B52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3094,19 +3095,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3126,7 +3127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3146,7 +3147,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3166,7 +3167,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3186,7 +3187,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3206,7 +3207,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3226,7 +3227,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3246,7 +3247,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3266,7 +3267,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3286,7 +3287,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3306,7 +3307,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3326,7 +3327,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3346,7 +3347,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3366,7 +3367,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3386,7 +3387,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3406,7 +3407,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3426,7 +3427,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3446,7 +3447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3466,7 +3467,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3486,7 +3487,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3506,7 +3507,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3526,7 +3527,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3546,7 +3547,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3566,7 +3567,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3586,7 +3587,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3606,7 +3607,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3626,7 +3627,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3646,7 +3647,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3666,7 +3667,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3686,7 +3687,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3706,7 +3707,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3726,7 +3727,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3746,7 +3747,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3766,7 +3767,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3786,7 +3787,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3806,7 +3807,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3826,7 +3827,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3846,7 +3847,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3866,7 +3867,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3886,7 +3887,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3906,7 +3907,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3926,7 +3927,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3946,7 +3947,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3966,7 +3967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3986,7 +3987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4006,7 +4007,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4026,7 +4027,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4046,7 +4047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4066,7 +4067,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4086,7 +4087,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4106,7 +4107,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4126,7 +4127,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4146,7 +4147,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4167,7 +4168,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:D53">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D53">
     <sortCondition ref="B2:B53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4175,19 +4176,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4207,7 +4208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4227,7 +4228,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4247,7 +4248,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4267,7 +4268,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4287,7 +4288,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4307,7 +4308,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4327,7 +4328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4347,7 +4348,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4367,7 +4368,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4387,7 +4388,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4407,7 +4408,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4427,7 +4428,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4447,7 +4448,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4467,7 +4468,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4487,7 +4488,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4507,7 +4508,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4527,7 +4528,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4547,7 +4548,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4567,7 +4568,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4587,7 +4588,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4607,7 +4608,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4627,7 +4628,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4647,7 +4648,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4667,7 +4668,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4687,7 +4688,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4707,7 +4708,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4727,7 +4728,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4747,7 +4748,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4767,7 +4768,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4787,7 +4788,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4807,7 +4808,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4827,7 +4828,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4847,7 +4848,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4867,7 +4868,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4887,7 +4888,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4907,7 +4908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4927,7 +4928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4947,7 +4948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4967,7 +4968,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4987,7 +4988,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5007,7 +5008,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5027,7 +5028,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5047,7 +5048,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5067,7 +5068,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5087,7 +5088,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5107,7 +5108,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5127,7 +5128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5147,7 +5148,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5167,7 +5168,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5188,7 +5189,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:D50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D50">
     <sortCondition ref="B2:B50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>